<commit_message>
all code for the draft
</commit_message>
<xml_diff>
--- a/Datasets/Riskperceptiondataset_201125.xlsx
+++ b/Datasets/Riskperceptiondataset_201125.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ca3652908a58f1c/BEP/BranchInes/Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/idattatreya_tudelft_nl/Documents/BEP/BranchInes/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23BA4258-C1F5-494F-94D9-488904206FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{23BA4258-C1F5-494F-94D9-488904206FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{669F39C9-699E-4637-98FA-557A77438F0E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllsurveyforLCA" sheetId="3" r:id="rId1"/>
@@ -569,7 +569,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,7 +632,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -645,6 +645,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -936,18 +940,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043D802E-6803-430C-9369-26993460540E}">
   <dimension ref="A1:X160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="72" workbookViewId="0">
       <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.703125" customWidth="1"/>
+    <col min="2" max="2" width="10.703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.703125" customWidth="1"/>
+    <col min="23" max="23" width="14.41015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1026,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1092,7 +1097,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1163,7 +1168,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1234,7 +1239,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1305,7 +1310,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1376,7 +1381,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1447,7 +1452,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1518,7 +1523,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1589,7 +1594,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1660,7 +1665,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1731,7 +1736,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1802,7 +1807,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1873,7 +1878,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1944,7 +1949,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2015,7 +2020,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2086,7 +2091,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2157,7 +2162,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2228,7 +2233,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2299,7 +2304,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2370,7 +2375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2441,7 +2446,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2512,7 +2517,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2583,7 +2588,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2654,7 +2659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2725,7 +2730,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2796,7 +2801,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2867,7 +2872,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2938,7 +2943,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3009,7 +3014,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3080,7 +3085,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3151,7 +3156,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3222,7 +3227,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3293,7 +3298,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3364,7 +3369,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3435,7 +3440,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3506,7 +3511,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3577,7 +3582,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3648,7 +3653,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3719,7 +3724,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3790,7 +3795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3861,7 +3866,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3932,7 +3937,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4003,7 +4008,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4074,7 +4079,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4145,7 +4150,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:23">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4216,7 +4221,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4287,7 +4292,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4358,7 +4363,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:23">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4429,7 +4434,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:23">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4500,7 +4505,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4571,7 +4576,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4642,7 +4647,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4713,7 +4718,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4784,7 +4789,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:23">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4855,7 +4860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:23">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4926,7 +4931,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:23">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4997,7 +5002,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:23">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5068,7 +5073,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5139,7 +5144,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:23">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5210,7 +5215,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5281,7 +5286,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5352,7 +5357,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5423,7 +5428,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:23">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5494,7 +5499,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:23">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5565,7 +5570,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:23">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5636,7 +5641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:23">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5707,7 +5712,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:23">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5778,7 +5783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="1:23">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5849,7 +5854,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:23">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5920,7 +5925,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:23">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5991,7 +5996,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:23">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6062,7 +6067,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:23">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6133,7 +6138,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:23">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6204,7 +6209,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:23">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6275,7 +6280,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:23">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6346,7 +6351,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="77" spans="1:23">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6417,7 +6422,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:23">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6488,7 +6493,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:23">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6559,7 +6564,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:23">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A80">
         <f>A79+1</f>
         <v>79</v>
@@ -6631,7 +6636,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="1:23">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A81">
         <f>A80+1</f>
         <v>80</v>
@@ -6703,7 +6708,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:23">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A82">
         <f t="shared" ref="A82:A145" si="0">A81+1</f>
         <v>81</v>
@@ -6775,7 +6780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:23">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A83">
         <f t="shared" si="0"/>
         <v>82</v>
@@ -6847,7 +6852,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="84" spans="1:23">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A84">
         <f t="shared" si="0"/>
         <v>83</v>
@@ -6919,7 +6924,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:23">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A85">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -6991,7 +6996,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:23">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A86">
         <f t="shared" si="0"/>
         <v>85</v>
@@ -7063,7 +7068,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="1:23">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A87">
         <f t="shared" si="0"/>
         <v>86</v>
@@ -7135,7 +7140,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:23">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A88">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -7207,7 +7212,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:23">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A89">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -7279,7 +7284,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:23">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A90">
         <f t="shared" si="0"/>
         <v>89</v>
@@ -7351,7 +7356,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="91" spans="1:23">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A91">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -7423,7 +7428,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:23">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A92">
         <f t="shared" si="0"/>
         <v>91</v>
@@ -7495,7 +7500,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:23">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A93">
         <f t="shared" si="0"/>
         <v>92</v>
@@ -7567,7 +7572,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:23">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A94">
         <f t="shared" si="0"/>
         <v>93</v>
@@ -7639,7 +7644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:23">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A95">
         <f t="shared" si="0"/>
         <v>94</v>
@@ -7711,7 +7716,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:23">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A96">
         <f t="shared" si="0"/>
         <v>95</v>
@@ -7783,7 +7788,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:23">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A97">
         <f t="shared" si="0"/>
         <v>96</v>
@@ -7855,7 +7860,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="98" spans="1:23">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A98">
         <f t="shared" si="0"/>
         <v>97</v>
@@ -7927,7 +7932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="99" spans="1:23">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A99">
         <f t="shared" si="0"/>
         <v>98</v>
@@ -7999,7 +8004,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="100" spans="1:23">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A100">
         <f t="shared" si="0"/>
         <v>99</v>
@@ -8071,7 +8076,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="1:23">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A101">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -8143,7 +8148,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="102" spans="1:23">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A102">
         <f t="shared" si="0"/>
         <v>101</v>
@@ -8215,7 +8220,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:23">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A103">
         <f t="shared" si="0"/>
         <v>102</v>
@@ -8287,7 +8292,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:23">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A104">
         <f t="shared" si="0"/>
         <v>103</v>
@@ -8359,7 +8364,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="105" spans="1:23">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A105">
         <f t="shared" si="0"/>
         <v>104</v>
@@ -8431,7 +8436,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="106" spans="1:23">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A106">
         <f t="shared" si="0"/>
         <v>105</v>
@@ -8446,7 +8451,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="1:23">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A107">
         <f t="shared" si="0"/>
         <v>106</v>
@@ -8518,7 +8523,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="108" spans="1:23">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A108">
         <f t="shared" si="0"/>
         <v>107</v>
@@ -8590,7 +8595,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="109" spans="1:23">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A109">
         <f t="shared" si="0"/>
         <v>108</v>
@@ -8662,7 +8667,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="1:23">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A110">
         <f t="shared" si="0"/>
         <v>109</v>
@@ -8734,7 +8739,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="111" spans="1:23">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A111">
         <f t="shared" si="0"/>
         <v>110</v>
@@ -8806,7 +8811,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="112" spans="1:23">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A112">
         <f t="shared" si="0"/>
         <v>111</v>
@@ -8878,7 +8883,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="113" spans="1:23">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A113">
         <f t="shared" si="0"/>
         <v>112</v>
@@ -8950,7 +8955,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="114" spans="1:23">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A114">
         <f t="shared" si="0"/>
         <v>113</v>
@@ -9022,7 +9027,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="115" spans="1:23">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A115">
         <f t="shared" si="0"/>
         <v>114</v>
@@ -9094,7 +9099,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="116" spans="1:23">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A116">
         <f t="shared" si="0"/>
         <v>115</v>
@@ -9166,7 +9171,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:23">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A117">
         <f t="shared" si="0"/>
         <v>116</v>
@@ -9238,7 +9243,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="118" spans="1:23">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A118">
         <f t="shared" si="0"/>
         <v>117</v>
@@ -9310,7 +9315,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="1:23">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A119">
         <f t="shared" si="0"/>
         <v>118</v>
@@ -9382,7 +9387,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="120" spans="1:23">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A120">
         <f t="shared" si="0"/>
         <v>119</v>
@@ -9454,7 +9459,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="121" spans="1:23">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A121">
         <f t="shared" si="0"/>
         <v>120</v>
@@ -9526,7 +9531,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="122" spans="1:23">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A122">
         <f t="shared" si="0"/>
         <v>121</v>
@@ -9598,7 +9603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="123" spans="1:23">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A123">
         <f t="shared" si="0"/>
         <v>122</v>
@@ -9670,7 +9675,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:23">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A124">
         <f t="shared" si="0"/>
         <v>123</v>
@@ -9742,7 +9747,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="125" spans="1:23">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A125">
         <f t="shared" si="0"/>
         <v>124</v>
@@ -9814,7 +9819,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:23">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A126">
         <f t="shared" si="0"/>
         <v>125</v>
@@ -9886,7 +9891,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="1:23">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A127">
         <f t="shared" si="0"/>
         <v>126</v>
@@ -9958,7 +9963,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="128" spans="1:23">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A128">
         <f t="shared" si="0"/>
         <v>127</v>
@@ -10030,7 +10035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:23">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A129">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -10102,7 +10107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="130" spans="1:23">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A130">
         <f t="shared" si="0"/>
         <v>129</v>
@@ -10174,7 +10179,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="1:23">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A131">
         <f t="shared" si="0"/>
         <v>130</v>
@@ -10246,7 +10251,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:23">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A132">
         <f t="shared" si="0"/>
         <v>131</v>
@@ -10315,7 +10320,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:23">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A133">
         <f t="shared" si="0"/>
         <v>132</v>
@@ -10387,7 +10392,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="134" spans="1:23">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A134">
         <f t="shared" si="0"/>
         <v>133</v>
@@ -10459,7 +10464,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:23">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A135">
         <f t="shared" si="0"/>
         <v>134</v>
@@ -10531,7 +10536,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="136" spans="1:23">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A136">
         <f t="shared" si="0"/>
         <v>135</v>
@@ -10603,7 +10608,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="137" spans="1:23">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A137">
         <f t="shared" si="0"/>
         <v>136</v>
@@ -10675,7 +10680,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="138" spans="1:23">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A138">
         <f t="shared" si="0"/>
         <v>137</v>
@@ -10747,7 +10752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="139" spans="1:23">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A139">
         <f t="shared" si="0"/>
         <v>138</v>
@@ -10819,7 +10824,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="140" spans="1:23">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A140">
         <f t="shared" si="0"/>
         <v>139</v>
@@ -10891,7 +10896,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="141" spans="1:23">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A141">
         <f t="shared" si="0"/>
         <v>140</v>
@@ -10963,7 +10968,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="142" spans="1:23">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A142">
         <f t="shared" si="0"/>
         <v>141</v>
@@ -11035,7 +11040,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="143" spans="1:23">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A143">
         <f t="shared" si="0"/>
         <v>142</v>
@@ -11107,7 +11112,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="144" spans="1:23">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A144">
         <f t="shared" si="0"/>
         <v>143</v>
@@ -11179,7 +11184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="145" spans="1:23">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A145">
         <f t="shared" si="0"/>
         <v>144</v>
@@ -11251,7 +11256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="146" spans="1:23">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A146">
         <f t="shared" ref="A146:A154" si="1">A145+1</f>
         <v>145</v>
@@ -11323,7 +11328,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:23">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A147">
         <f t="shared" si="1"/>
         <v>146</v>
@@ -11395,7 +11400,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="148" spans="1:23">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A148">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -11467,7 +11472,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="149" spans="1:23">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A149">
         <f t="shared" si="1"/>
         <v>148</v>
@@ -11539,7 +11544,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="1:23">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A150">
         <f t="shared" si="1"/>
         <v>149</v>
@@ -11611,7 +11616,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="151" spans="1:23">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A151">
         <f t="shared" si="1"/>
         <v>150</v>
@@ -11683,7 +11688,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="152" spans="1:23">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A152">
         <f t="shared" si="1"/>
         <v>151</v>
@@ -11755,7 +11760,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="153" spans="1:23">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A153">
         <f t="shared" si="1"/>
         <v>152</v>
@@ -11827,7 +11832,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="154" spans="1:23">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A154">
         <f t="shared" si="1"/>
         <v>153</v>
@@ -11899,13 +11904,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="158" spans="1:23">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.5">
       <c r="B158" s="6"/>
     </row>
-    <row r="159" spans="1:23">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.5">
       <c r="B159" s="6"/>
     </row>
-    <row r="160" spans="1:23">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.5">
       <c r="B160" s="6"/>
     </row>
   </sheetData>
@@ -11921,14 +11926,17 @@
       <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="16.5859375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="B1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>167</v>
       </c>
@@ -11936,7 +11944,7 @@
         <v>45559</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -11944,7 +11952,7 @@
         <v>45923</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -11961,19 +11969,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F58E04D-405E-46DC-8E26-3872CFE84DE0}">
   <dimension ref="A1:AA156"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="65" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScale="65" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="22" max="22" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.703125" customWidth="1"/>
+    <col min="3" max="3" width="29.29296875" customWidth="1"/>
+    <col min="4" max="4" width="21.29296875" customWidth="1"/>
+    <col min="22" max="22" width="12.29296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12044,7 +12052,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12115,7 +12123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12186,7 +12194,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12257,7 +12265,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12328,7 +12336,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -12399,7 +12407,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -12470,7 +12478,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -12541,7 +12549,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -12612,7 +12620,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -12683,7 +12691,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -12754,7 +12762,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -12825,7 +12833,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -12896,7 +12904,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -12967,7 +12975,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -13038,7 +13046,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -13109,7 +13117,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>16</v>
       </c>
@@ -13180,7 +13188,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>17</v>
       </c>
@@ -13251,7 +13259,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>18</v>
       </c>
@@ -13322,7 +13330,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>19</v>
       </c>
@@ -13393,7 +13401,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>20</v>
       </c>
@@ -13464,7 +13472,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>21</v>
       </c>
@@ -13535,7 +13543,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>22</v>
       </c>
@@ -13606,7 +13614,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>23</v>
       </c>
@@ -13677,7 +13685,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>24</v>
       </c>
@@ -13748,7 +13756,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -13819,7 +13827,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>26</v>
       </c>
@@ -13890,7 +13898,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>27</v>
       </c>
@@ -13961,7 +13969,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>28</v>
       </c>
@@ -14032,7 +14040,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>29</v>
       </c>
@@ -14103,7 +14111,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>30</v>
       </c>
@@ -14174,7 +14182,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>31</v>
       </c>
@@ -14245,7 +14253,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>32</v>
       </c>
@@ -14316,7 +14324,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>33</v>
       </c>
@@ -14387,7 +14395,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>34</v>
       </c>
@@ -14458,7 +14466,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>35</v>
       </c>
@@ -14529,7 +14537,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>36</v>
       </c>
@@ -14600,7 +14608,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>37</v>
       </c>
@@ -14671,7 +14679,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>38</v>
       </c>
@@ -14742,7 +14750,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>39</v>
       </c>
@@ -14813,7 +14821,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>40</v>
       </c>
@@ -14884,7 +14892,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>41</v>
       </c>
@@ -14955,7 +14963,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>42</v>
       </c>
@@ -15026,7 +15034,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>43</v>
       </c>
@@ -15097,7 +15105,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>44</v>
       </c>
@@ -15168,7 +15176,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:23">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>45</v>
       </c>
@@ -15239,7 +15247,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>46</v>
       </c>
@@ -15310,7 +15318,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>47</v>
       </c>
@@ -15381,7 +15389,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:23">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>48</v>
       </c>
@@ -15452,7 +15460,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:23">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>49</v>
       </c>
@@ -15523,7 +15531,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>50</v>
       </c>
@@ -15594,7 +15602,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>51</v>
       </c>
@@ -15665,7 +15673,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>52</v>
       </c>
@@ -15736,7 +15744,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>53</v>
       </c>
@@ -15807,7 +15815,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:23">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>54</v>
       </c>
@@ -15878,7 +15886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:23">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>55</v>
       </c>
@@ -15949,7 +15957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:23">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>56</v>
       </c>
@@ -16020,7 +16028,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:23">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>57</v>
       </c>
@@ -16091,7 +16099,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>58</v>
       </c>
@@ -16162,7 +16170,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:23">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>59</v>
       </c>
@@ -16233,7 +16241,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>60</v>
       </c>
@@ -16304,7 +16312,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>61</v>
       </c>
@@ -16375,7 +16383,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>62</v>
       </c>
@@ -16446,7 +16454,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:23">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>63</v>
       </c>
@@ -16517,7 +16525,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:27">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>64</v>
       </c>
@@ -16588,7 +16596,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:27">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>65</v>
       </c>
@@ -16659,7 +16667,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:27">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>66</v>
       </c>
@@ -16730,7 +16738,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:27">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>67</v>
       </c>
@@ -16801,7 +16809,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="1:27">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>68</v>
       </c>
@@ -16872,7 +16880,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:27">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>69</v>
       </c>
@@ -16943,7 +16951,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:27">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>70</v>
       </c>
@@ -17014,7 +17022,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:27">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A72">
         <v>71</v>
       </c>
@@ -17085,7 +17093,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:27">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A73">
         <v>72</v>
       </c>
@@ -17156,7 +17164,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:27">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A74">
         <v>73</v>
       </c>
@@ -17227,7 +17235,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:27">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A75">
         <v>74</v>
       </c>
@@ -17298,7 +17306,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:27">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A76">
         <v>75</v>
       </c>
@@ -17369,7 +17377,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="77" spans="1:27">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>76</v>
       </c>
@@ -17440,7 +17448,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:27">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>77</v>
       </c>
@@ -17511,7 +17519,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:27">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A79">
         <v>78</v>
       </c>
@@ -17582,7 +17590,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:27">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -17665,7 +17673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A81">
         <v>1</v>
       </c>
@@ -17748,7 +17756,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A82">
         <v>2</v>
       </c>
@@ -17831,7 +17839,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A83">
         <v>3</v>
       </c>
@@ -17914,7 +17922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A84">
         <v>4</v>
       </c>
@@ -17997,7 +18005,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A85">
         <v>5</v>
       </c>
@@ -18080,7 +18088,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A86">
         <v>6</v>
       </c>
@@ -18163,7 +18171,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A87">
         <v>7</v>
       </c>
@@ -18246,7 +18254,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A88">
         <v>8</v>
       </c>
@@ -18329,7 +18337,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A89">
         <v>9</v>
       </c>
@@ -18412,7 +18420,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A90">
         <v>10</v>
       </c>
@@ -18495,7 +18503,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A91">
         <v>11</v>
       </c>
@@ -18578,7 +18586,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A92">
         <v>12</v>
       </c>
@@ -18661,7 +18669,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A93">
         <v>13</v>
       </c>
@@ -18744,7 +18752,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A94">
         <v>14</v>
       </c>
@@ -18827,7 +18835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A95">
         <v>15</v>
       </c>
@@ -18910,7 +18918,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A96">
         <v>16</v>
       </c>
@@ -18993,7 +19001,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="97" spans="1:27">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A97">
         <v>17</v>
       </c>
@@ -19076,7 +19084,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:27">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A98">
         <v>18</v>
       </c>
@@ -19159,7 +19167,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="99" spans="1:27">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A99">
         <v>19</v>
       </c>
@@ -19242,7 +19250,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:27">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A100">
         <v>20</v>
       </c>
@@ -19325,7 +19333,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="1:27">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A101">
         <v>21</v>
       </c>
@@ -19408,7 +19416,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="102" spans="1:27">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A102">
         <v>22</v>
       </c>
@@ -19491,7 +19499,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:27">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A103">
         <v>23</v>
       </c>
@@ -19574,7 +19582,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:27">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A104">
         <v>24</v>
       </c>
@@ -19657,7 +19665,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="105" spans="1:27">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A105">
         <v>25</v>
       </c>
@@ -19740,7 +19748,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="106" spans="1:27">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A106">
         <v>26</v>
       </c>
@@ -19823,7 +19831,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="1:27">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A107">
         <v>27</v>
       </c>
@@ -19841,7 +19849,7 @@
       <c r="T107" s="5"/>
       <c r="U107" s="5"/>
     </row>
-    <row r="108" spans="1:27">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A108">
         <v>28</v>
       </c>
@@ -19924,7 +19932,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="109" spans="1:27">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A109">
         <v>29</v>
       </c>
@@ -20007,7 +20015,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="110" spans="1:27">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A110">
         <v>30</v>
       </c>
@@ -20090,7 +20098,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="1:27">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A111">
         <v>31</v>
       </c>
@@ -20173,7 +20181,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="112" spans="1:27">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A112">
         <v>32</v>
       </c>
@@ -20256,7 +20264,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:27">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A113">
         <v>33</v>
       </c>
@@ -20335,7 +20343,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:27">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A114">
         <v>34</v>
       </c>
@@ -20418,7 +20426,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="115" spans="1:27">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A115">
         <v>35</v>
       </c>
@@ -20501,7 +20509,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="116" spans="1:27">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A116">
         <v>36</v>
       </c>
@@ -20584,7 +20592,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="117" spans="1:27">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A117">
         <v>37</v>
       </c>
@@ -20667,7 +20675,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="118" spans="1:27">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A118">
         <v>38</v>
       </c>
@@ -20750,7 +20758,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="1:27">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A119">
         <v>39</v>
       </c>
@@ -20833,7 +20841,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="120" spans="1:27">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A120">
         <v>40</v>
       </c>
@@ -20916,7 +20924,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="1:27">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A121">
         <v>41</v>
       </c>
@@ -20999,7 +21007,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="122" spans="1:27">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A122">
         <v>42</v>
       </c>
@@ -21082,7 +21090,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="123" spans="1:27">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A123">
         <v>43</v>
       </c>
@@ -21165,7 +21173,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="124" spans="1:27">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A124">
         <v>44</v>
       </c>
@@ -21248,7 +21256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:27">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A125">
         <v>45</v>
       </c>
@@ -21331,7 +21339,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="126" spans="1:27">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A126">
         <v>46</v>
       </c>
@@ -21414,7 +21422,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:27">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A127">
         <v>47</v>
       </c>
@@ -21497,7 +21505,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="128" spans="1:27">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A128">
         <v>48</v>
       </c>
@@ -21580,7 +21588,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="129" spans="1:27">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A129">
         <v>49</v>
       </c>
@@ -21663,7 +21671,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="130" spans="1:27">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A130">
         <v>50</v>
       </c>
@@ -21746,7 +21754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="131" spans="1:27">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A131">
         <v>51</v>
       </c>
@@ -21829,7 +21837,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:27">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A132">
         <v>52</v>
       </c>
@@ -21912,7 +21920,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:27">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A133" s="1" t="s">
         <v>0</v>
       </c>
@@ -21995,7 +22003,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="134" spans="1:27">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A134">
         <v>1</v>
       </c>
@@ -22075,7 +22083,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:27">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A135">
         <v>2</v>
       </c>
@@ -22158,7 +22166,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="136" spans="1:27">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A136">
         <v>3</v>
       </c>
@@ -22241,7 +22249,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="137" spans="1:27">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A137">
         <v>4</v>
       </c>
@@ -22324,7 +22332,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="138" spans="1:27">
+    <row r="138" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A138">
         <v>5</v>
       </c>
@@ -22407,7 +22415,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="139" spans="1:27">
+    <row r="139" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A139">
         <v>6</v>
       </c>
@@ -22490,7 +22498,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="140" spans="1:27">
+    <row r="140" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A140">
         <v>7</v>
       </c>
@@ -22573,7 +22581,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="141" spans="1:27">
+    <row r="141" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A141">
         <v>8</v>
       </c>
@@ -22656,7 +22664,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="142" spans="1:27">
+    <row r="142" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A142">
         <v>9</v>
       </c>
@@ -22739,7 +22747,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:27">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A143">
         <v>10</v>
       </c>
@@ -22822,7 +22830,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="144" spans="1:27">
+    <row r="144" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A144">
         <v>11</v>
       </c>
@@ -22905,7 +22913,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="145" spans="1:27">
+    <row r="145" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A145">
         <v>12</v>
       </c>
@@ -22988,7 +22996,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="146" spans="1:27">
+    <row r="146" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A146">
         <v>13</v>
       </c>
@@ -23071,7 +23079,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:27">
+    <row r="147" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A147">
         <v>14</v>
       </c>
@@ -23154,7 +23162,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="148" spans="1:27">
+    <row r="148" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A148">
         <v>15</v>
       </c>
@@ -23237,7 +23245,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="149" spans="1:27">
+    <row r="149" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A149">
         <v>16</v>
       </c>
@@ -23320,7 +23328,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="1:27">
+    <row r="150" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A150">
         <v>17</v>
       </c>
@@ -23403,7 +23411,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="151" spans="1:27">
+    <row r="151" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A151">
         <v>18</v>
       </c>
@@ -23486,7 +23494,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="152" spans="1:27">
+    <row r="152" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A152">
         <v>19</v>
       </c>
@@ -23569,7 +23577,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="153" spans="1:27">
+    <row r="153" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A153">
         <v>20</v>
       </c>
@@ -23652,7 +23660,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="154" spans="1:27">
+    <row r="154" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A154">
         <v>21</v>
       </c>
@@ -23735,7 +23743,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="155" spans="1:27">
+    <row r="155" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A155">
         <v>22</v>
       </c>
@@ -23818,7 +23826,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="156" spans="1:27">
+    <row r="156" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A156">
         <v>23</v>
       </c>

</xml_diff>